<commit_message>
allowance on the tire s8
</commit_message>
<xml_diff>
--- a/Контрольная ведомость Заказ №1.xlsx.xlsx
+++ b/Контрольная ведомость Заказ №1.xlsx.xlsx
@@ -423,7 +423,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -489,7 +489,7 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>E3-55-Al-1000-4-pt3.0</t>
+          <t>E3-55-Al-5000-3-uv</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
@@ -499,55 +499,25 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>прямая секция</t>
+          <t>угловая вертикальная секция</t>
         </is>
       </c>
       <c r="E2" s="2" t="inlineStr">
         <is>
-          <t>3000</t>
+          <t>450х450</t>
         </is>
       </c>
       <c r="F2" s="2" t="inlineStr"/>
       <c r="I2" s="2" t="n">
-        <v>32.40000000000001</v>
+        <v>41.94</v>
       </c>
       <c r="J2" s="2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t>E3-55-Al-1250-4-pt3.0</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>1-1-0002</t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="inlineStr">
-        <is>
-          <t>прямая секция</t>
-        </is>
-      </c>
-      <c r="E3" s="2" t="inlineStr">
-        <is>
-          <t>3000</t>
-        </is>
-      </c>
-      <c r="F3" s="2" t="inlineStr"/>
-      <c r="I3" s="2" t="n">
-        <v>39.6</v>
-      </c>
-      <c r="J3" s="2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup fitToHeight="0"/>
   <headerFooter>
-    <oddHeader>&amp;L&amp;"Century Gothic"&amp;12 Заказ № 1&amp;C&amp;"Century Gothic"&amp;20 Упаковка&amp;R&amp;"Century Gothic"&amp;12 ООО «ПИК «СОЛЯРИС»_x000a_11 10 2021</oddHeader>
+    <oddHeader>&amp;L&amp;"Century Gothic"&amp;12 Заказ № 1&amp;C&amp;"Century Gothic"&amp;20 Упаковка&amp;R&amp;"Century Gothic"&amp;12 ООО «ПИК «СОЛЯРИС»_x000a_21 10 2021</oddHeader>
     <oddFooter>&amp;R&amp;"Century Gothic"&amp;10 №3818_x000a_EEk</oddFooter>
     <evenHeader/>
     <evenFooter/>

</xml_diff>